<commit_message>
feat: add tableau compiler 'tableauc' to generate protoconf
</commit_message>
<xml_diff>
--- a/test/testdata/hero/Test.xlsx
+++ b/test/testdata/hero/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\hero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E73326-EA42-4674-B3D4-B95AFCED84A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E19380-3B87-4249-8C98-4AEC2CBA21BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="5460" windowWidth="38670" windowHeight="14295" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="10905" yWindow="5640" windowWidth="38670" windowHeight="14295" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hero" sheetId="7" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>